<commit_message>
Slide added for rastrigin function and filled test cases in excel file.
</commit_message>
<xml_diff>
--- a/Code/TestValues.xlsx
+++ b/Code/TestValues.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shalin\Desktop\project-pyteam\Code\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TestValues" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,13 +21,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>w</t>
+    <t>Num_Iterations</t>
   </si>
   <si>
-    <t>c1</t>
+    <t>Num_dimesdions</t>
   </si>
   <si>
-    <t>c2</t>
+    <t>Num_Particles</t>
   </si>
 </sst>
 </file>
@@ -131,7 +126,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -166,7 +161,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -343,7 +338,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -351,23 +346,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1">
+        <v>10</v>
+      </c>
+      <c r="C1">
+        <v>20</v>
+      </c>
+      <c r="D1">
+        <v>30</v>
+      </c>
+      <c r="E1">
+        <v>40</v>
+      </c>
+      <c r="F1">
+        <v>50</v>
+      </c>
+      <c r="G1">
+        <v>60</v>
+      </c>
+      <c r="H1">
+        <v>70</v>
+      </c>
+      <c r="I1">
+        <v>80</v>
+      </c>
+      <c r="J1">
+        <v>90</v>
+      </c>
+      <c r="K1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>200</v>
+      </c>
+      <c r="D2">
+        <v>300</v>
+      </c>
+      <c r="E2">
+        <v>400</v>
+      </c>
+      <c r="F2">
+        <v>500</v>
+      </c>
+      <c r="G2">
+        <v>600</v>
+      </c>
+      <c r="H2">
+        <v>700</v>
+      </c>
+      <c r="I2">
+        <v>800</v>
+      </c>
+      <c r="J2">
+        <v>900</v>
+      </c>
+      <c r="K2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B3">
         <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>7</v>
+      </c>
+      <c r="H3">
+        <v>8</v>
+      </c>
+      <c r="I3">
+        <v>9</v>
+      </c>
+      <c r="J3">
+        <v>10</v>
+      </c>
+      <c r="K3">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>